<commit_message>
changes, database upload still broken
</commit_message>
<xml_diff>
--- a/dev_database/Travel Event Dashboard_DATA_20 Feb_fixed.xlsx
+++ b/dev_database/Travel Event Dashboard_DATA_20 Feb_fixed.xlsx
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Travel Event Dashboard DATA'!$A$2:$L$79</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Travel Event Dashboard DATA'!$A$2:$L$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Travel Event Dashboard DATA'!$A$2:$L$79</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="213">
   <si>
     <t xml:space="preserve">TRAVELERS: This is the person traveling and their organization.  The system will guess and flag people from WBG based on orgainzational value (eg, 'World Bank' 'IFC' 'MIGA' 'IBRD').  These underlined fields are required</t>
   </si>
@@ -959,24 +960,24 @@
   </sheetPr>
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G79" activeCellId="0" sqref="G79"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9642857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.0969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.219387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.8928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="28.5357142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="47.2091836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="14.1938775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.4948979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="27.6173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="45.6632653061225"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="13.5816326530612"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.0459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.86734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="87.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3193,7 +3194,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>25</v>
       </c>
@@ -3216,9 +3217,7 @@
         <v>202</v>
       </c>
       <c r="H81" s="2"/>
-      <c r="I81" s="0" t="s">
-        <v>202</v>
-      </c>
+      <c r="I81" s="0"/>
       <c r="J81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>